<commit_message>
Add PROJECT_ID column with values to sub files
Project identifier is required information for invoices. This change
adds a column titled PROJECT_ID to the example subcontractor files with
example values
</commit_message>
<xml_diff>
--- a/sub_folder/finn.xlsx
+++ b/sub_folder/finn.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry\Desktop\invoices-suck\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry\Desktop\invoices-suck\sub_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153E1E92-4646-42BF-8040-433C99654DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DAADE8-4FF2-4121-A1B2-E61711C2CE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28500" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2532" yWindow="2532" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="31">
   <si>
     <t>BILL_DATE</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>Kick</t>
+  </si>
+  <si>
+    <t>PROJECT_ID</t>
+  </si>
+  <si>
+    <t>Candy_kingdom</t>
+  </si>
+  <si>
+    <t>Nightosphere</t>
+  </si>
+  <si>
+    <t>Treehouse</t>
   </si>
 </sst>
 </file>
@@ -453,20 +465,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="12.68359375" customWidth="1"/>
     <col min="2" max="2" width="12.83984375" customWidth="1"/>
-    <col min="5" max="5" width="105.734375" customWidth="1"/>
+    <col min="3" max="3" width="14.5234375" customWidth="1"/>
+    <col min="6" max="6" width="105.734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -474,352 +487,412 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3">
         <v>45108</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>0.5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3">
         <v>45109</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>0.5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>45110</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>45112</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>0.5</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>45115</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="4">
         <v>0.5</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>45115</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>45117</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="4">
         <v>0.5</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>45136</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="4">
         <v>2.5</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>45119</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="4">
         <v>4</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>45126</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="4">
         <v>2</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>45110</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="4">
         <v>2.5</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3">
         <v>45110</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="4">
         <v>2</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
         <v>45129</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="4">
+      <c r="E14" s="4">
         <v>1</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3">
         <v>45121</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="4">
         <v>2</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3">
         <v>45110</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="4">
         <v>2</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="F16" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3">
         <v>45110</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="4">
+      <c r="E17" s="4">
         <v>2.5</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3">
         <v>45127</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="4">
+      <c r="E18" s="4">
         <v>2</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3">
         <v>45120</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="4">
+      <c r="E19" s="4">
         <v>2</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="F19" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3">
         <v>45120</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="4">
+      <c r="E20" s="4">
         <v>2.5</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="F20" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>